<commit_message>
Actualizacion de datos y ajustes en el codigo
</commit_message>
<xml_diff>
--- a/CasosCancer-Guaranis.xlsx
+++ b/CasosCancer-Guaranis.xlsx
@@ -6,26 +6,22 @@
     <sheet state="visible" name="CANCER-C" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="CANCER-G" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="CANCER-L" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="CANCER-PC" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="CANCER-SC" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="CANCER-R-C" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="CANCER-R-G" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="CANCER-R-L" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="CANCER-R-PC" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="CANCER-R-SC" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="CANCER-CV" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="CANCER-PC" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="CANCER-SC" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataChecksum="ni14icTJzFbzwoYpmcc4JS1nvyp7MW4Rsc3HoyOjljI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="HtiOcEDQQZqN97dC5+BBKwtCy/ntxS6bGZft/pidbtI="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="15">
   <si>
     <t>Año</t>
   </si>
@@ -76,9 +72,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d-m"/>
-  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11.0"/>
@@ -147,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -174,15 +167,6 @@
     </xf>
     <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -243,6 +227,11 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
+    <tableStyle count="3" pivot="0" name="CANCER-CV-style">
+      <tableStyleElement dxfId="1" type="headerRow"/>
+      <tableStyleElement dxfId="2" type="firstRowStripe"/>
+      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    </tableStyle>
     <tableStyle count="3" pivot="0" name="CANCER-PC-style">
       <tableStyleElement dxfId="1" type="headerRow"/>
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
@@ -253,20 +242,11 @@
       <tableStyleElement dxfId="2" type="firstRowStripe"/>
       <tableStyleElement dxfId="3" type="secondRowStripe"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="CANCER-R-G-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
-    </tableStyle>
   </tableStyles>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -287,18 +267,6 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -382,7 +350,7 @@
     <tableColumn name="60+" id="12"/>
     <tableColumn name="Total" id="13"/>
   </tableColumns>
-  <tableStyleInfo name="CANCER-PC-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="CANCER-CV-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -403,7 +371,7 @@
     <tableColumn name="60+" id="12"/>
     <tableColumn name="Total" id="13"/>
   </tableColumns>
-  <tableStyleInfo name="CANCER-SC-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="CANCER-PC-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -424,7 +392,7 @@
     <tableColumn name="60+" id="12"/>
     <tableColumn name="Total" id="13"/>
   </tableColumns>
-  <tableStyleInfo name="CANCER-R-G-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="CANCER-SC-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
 </table>
 </file>
 
@@ -1015,393 +983,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="26" width="8.43"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11">
-        <v>45383.0</v>
-      </c>
-      <c r="F1" s="11">
-        <v>45540.0</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>2020.0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5">
-        <v>5.0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>12.0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>63.0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>97.0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>87.0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>102.0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>314.0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>280.0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>554.0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>1215.0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>2729.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6">
-        <v>2020.0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8">
-        <v>17.0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>17.0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>77.0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>84.0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>106.0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>107.0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>852.0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>985.0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>915.0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1206.0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>4366.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>2021.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5">
-        <v>40.0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>28.0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>236.0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>294.0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>333.0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>173.0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>693.0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>783.0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1048.0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>2563.0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>6191.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6">
-        <v>2021.0</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8">
-        <v>57.0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>44.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>237.0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>294.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>318.0</v>
-      </c>
-      <c r="H5" s="8">
-        <v>356.0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>2660.0</v>
-      </c>
-      <c r="J5" s="8">
-        <v>3674.0</v>
-      </c>
-      <c r="K5" s="8">
-        <v>2850.0</v>
-      </c>
-      <c r="L5" s="8">
-        <v>3470.0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>13960.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3">
-        <v>2022.0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
-        <v>61.0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>44.0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>383.0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>454.0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>450.0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>387.0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1474.0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>1270.0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1729.0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>5674.0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>11926.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6">
-        <v>2022.0</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8">
-        <v>89.0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>99.0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>516.0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>366.0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>461.0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>406.0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>4930.0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>6931.0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>6162.0</v>
-      </c>
-      <c r="L7" s="8">
-        <v>8052.0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>28012.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <v>2023.0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5">
-        <v>85.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>81.0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>317.0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>289.0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>258.0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>270.0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1198.0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>931.0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>1552.0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>5119.0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>10100.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6">
-        <v>2023.0</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="8">
-        <v>209.0</v>
-      </c>
-      <c r="D9" s="8">
-        <v>185.0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>315.0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>267.0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>322.0</v>
-      </c>
-      <c r="H9" s="8">
-        <v>497.0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>4741.0</v>
-      </c>
-      <c r="J9" s="8">
-        <v>6373.0</v>
-      </c>
-      <c r="K9" s="8">
-        <v>4912.0</v>
-      </c>
-      <c r="L9" s="8">
-        <v>6865.0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>24686.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -2188,14 +1769,14 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <pageSetUpPr/>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="8.71"/>
+    <col customWidth="1" min="1" max="26" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2265,19 +1846,19 @@
         <v>0.0</v>
       </c>
       <c r="I2" s="5">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="J2" s="5">
         <v>0.0</v>
       </c>
       <c r="K2" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L2" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="M2" s="3">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -2306,19 +1887,19 @@
         <v>0.0</v>
       </c>
       <c r="I3" s="8">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J3" s="8">
         <v>0.0</v>
       </c>
       <c r="K3" s="8">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="L3" s="8">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="M3" s="6">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="4">
@@ -2353,13 +1934,13 @@
         <v>0.0</v>
       </c>
       <c r="K4" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="L4" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="3">
         <v>1.0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -2391,16 +1972,16 @@
         <v>0.0</v>
       </c>
       <c r="J5" s="8">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="K5" s="8">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="L5" s="8">
-        <v>6.0</v>
+        <v>0.0</v>
       </c>
       <c r="M5" s="6">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
@@ -2417,7 +1998,7 @@
         <v>0.0</v>
       </c>
       <c r="E6" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="F6" s="5">
         <v>0.0</v>
@@ -2426,22 +2007,22 @@
         <v>0.0</v>
       </c>
       <c r="H6" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I6" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="J6" s="5">
         <v>0.0</v>
       </c>
       <c r="K6" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="L6" s="5">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="M6" s="3">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
@@ -2470,19 +2051,19 @@
         <v>0.0</v>
       </c>
       <c r="I7" s="8">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="J7" s="8">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="K7" s="8">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="L7" s="8">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="M7" s="6">
-        <v>40.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -2508,22 +2089,22 @@
         <v>0.0</v>
       </c>
       <c r="H8" s="5">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="I8" s="5">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c r="J8" s="5">
         <v>0.0</v>
       </c>
       <c r="K8" s="5">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="L8" s="5">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="M8" s="3">
-        <v>21.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="9">
@@ -2552,25 +2133,22 @@
         <v>0.0</v>
       </c>
       <c r="I9" s="8">
-        <v>22.0</v>
+        <v>0.0</v>
       </c>
       <c r="J9" s="8">
-        <v>9.0</v>
+        <v>0.0</v>
       </c>
       <c r="K9" s="8">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c r="L9" s="8">
-        <v>8.0</v>
+        <v>0.0</v>
       </c>
       <c r="M9" s="6">
-        <v>43.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -2588,7 +2166,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="25" width="8.57"/>
+    <col customWidth="1" min="1" max="25" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2640,37 +2218,37 @@
         <v>13</v>
       </c>
       <c r="C2" s="5">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c r="D2" s="5">
-        <v>12.0</v>
+        <v>0.0</v>
       </c>
       <c r="E2" s="5">
-        <v>59.0</v>
+        <v>0.0</v>
       </c>
       <c r="F2" s="5">
-        <v>94.0</v>
+        <v>0.0</v>
       </c>
       <c r="G2" s="5">
-        <v>81.0</v>
+        <v>0.0</v>
       </c>
       <c r="H2" s="5">
-        <v>71.0</v>
+        <v>0.0</v>
       </c>
       <c r="I2" s="5">
-        <v>173.0</v>
+        <v>2.0</v>
       </c>
       <c r="J2" s="5">
-        <v>188.0</v>
+        <v>0.0</v>
       </c>
       <c r="K2" s="5">
-        <v>363.0</v>
+        <v>1.0</v>
       </c>
       <c r="L2" s="5">
-        <v>868.0</v>
+        <v>1.0</v>
       </c>
       <c r="M2" s="3">
-        <v>1914.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="3">
@@ -2681,37 +2259,37 @@
         <v>14</v>
       </c>
       <c r="C3" s="8">
-        <v>14.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" s="8">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="E3" s="8">
-        <v>71.0</v>
+        <v>0.0</v>
       </c>
       <c r="F3" s="8">
-        <v>72.0</v>
+        <v>0.0</v>
       </c>
       <c r="G3" s="8">
-        <v>91.0</v>
+        <v>0.0</v>
       </c>
       <c r="H3" s="8">
-        <v>78.0</v>
+        <v>0.0</v>
       </c>
       <c r="I3" s="8">
-        <v>636.0</v>
+        <v>1.0</v>
       </c>
       <c r="J3" s="8">
-        <v>669.0</v>
+        <v>0.0</v>
       </c>
       <c r="K3" s="8">
-        <v>601.0</v>
+        <v>3.0</v>
       </c>
       <c r="L3" s="8">
-        <v>747.0</v>
+        <v>2.0</v>
       </c>
       <c r="M3" s="6">
-        <v>2992.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="4">
@@ -2722,37 +2300,37 @@
         <v>13</v>
       </c>
       <c r="C4" s="5">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" s="5">
-        <v>23.0</v>
+        <v>0.0</v>
       </c>
       <c r="E4" s="5">
-        <v>206.0</v>
+        <v>1.0</v>
       </c>
       <c r="F4" s="5">
-        <v>261.0</v>
+        <v>0.0</v>
       </c>
       <c r="G4" s="5">
-        <v>280.0</v>
+        <v>0.0</v>
       </c>
       <c r="H4" s="5">
-        <v>126.0</v>
+        <v>0.0</v>
       </c>
       <c r="I4" s="5">
-        <v>468.0</v>
+        <v>0.0</v>
       </c>
       <c r="J4" s="5">
-        <v>546.0</v>
+        <v>0.0</v>
       </c>
       <c r="K4" s="5">
-        <v>704.0</v>
+        <v>1.0</v>
       </c>
       <c r="L4" s="5">
-        <v>1689.0</v>
+        <v>2.0</v>
       </c>
       <c r="M4" s="3">
-        <v>4338.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="5">
@@ -2763,37 +2341,37 @@
         <v>14</v>
       </c>
       <c r="C5" s="8">
-        <v>50.0</v>
+        <v>0.0</v>
       </c>
       <c r="D5" s="8">
-        <v>35.0</v>
+        <v>0.0</v>
       </c>
       <c r="E5" s="8">
-        <v>198.0</v>
+        <v>0.0</v>
       </c>
       <c r="F5" s="8">
-        <v>241.0</v>
+        <v>0.0</v>
       </c>
       <c r="G5" s="8">
-        <v>261.0</v>
+        <v>0.0</v>
       </c>
       <c r="H5" s="8">
-        <v>259.0</v>
+        <v>0.0</v>
       </c>
       <c r="I5" s="8">
-        <v>1911.0</v>
+        <v>0.0</v>
       </c>
       <c r="J5" s="8">
-        <v>2516.0</v>
+        <v>2.0</v>
       </c>
       <c r="K5" s="8">
-        <v>1773.0</v>
+        <v>12.0</v>
       </c>
       <c r="L5" s="8">
-        <v>2144.0</v>
+        <v>6.0</v>
       </c>
       <c r="M5" s="6">
-        <v>9388.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="6">
@@ -2804,37 +2382,37 @@
         <v>13</v>
       </c>
       <c r="C6" s="5">
-        <v>45.0</v>
+        <v>0.0</v>
       </c>
       <c r="D6" s="5">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="E6" s="5">
-        <v>351.0</v>
+        <v>1.0</v>
       </c>
       <c r="F6" s="5">
-        <v>428.0</v>
+        <v>0.0</v>
       </c>
       <c r="G6" s="5">
-        <v>408.0</v>
+        <v>0.0</v>
       </c>
       <c r="H6" s="5">
-        <v>302.0</v>
+        <v>1.0</v>
       </c>
       <c r="I6" s="5">
-        <v>950.0</v>
+        <v>1.0</v>
       </c>
       <c r="J6" s="5">
-        <v>770.0</v>
+        <v>0.0</v>
       </c>
       <c r="K6" s="5">
-        <v>1104.0</v>
+        <v>1.0</v>
       </c>
       <c r="L6" s="5">
-        <v>3605.0</v>
+        <v>5.0</v>
       </c>
       <c r="M6" s="3">
-        <v>7994.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="7">
@@ -2845,37 +2423,37 @@
         <v>14</v>
       </c>
       <c r="C7" s="8">
-        <v>71.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7" s="8">
-        <v>76.0</v>
+        <v>0.0</v>
       </c>
       <c r="E7" s="8">
-        <v>456.0</v>
+        <v>0.0</v>
       </c>
       <c r="F7" s="8">
-        <v>308.0</v>
+        <v>0.0</v>
       </c>
       <c r="G7" s="8">
-        <v>408.0</v>
+        <v>0.0</v>
       </c>
       <c r="H7" s="8">
-        <v>314.0</v>
+        <v>0.0</v>
       </c>
       <c r="I7" s="8">
-        <v>3315.0</v>
+        <v>10.0</v>
       </c>
       <c r="J7" s="8">
-        <v>4577.0</v>
+        <v>12.0</v>
       </c>
       <c r="K7" s="8">
-        <v>3760.0</v>
+        <v>9.0</v>
       </c>
       <c r="L7" s="8">
-        <v>4668.0</v>
+        <v>9.0</v>
       </c>
       <c r="M7" s="6">
-        <v>17953.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="8">
@@ -2886,37 +2464,37 @@
         <v>13</v>
       </c>
       <c r="C8" s="5">
-        <v>76.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8" s="5">
-        <v>68.0</v>
+        <v>0.0</v>
       </c>
       <c r="E8" s="5">
-        <v>218.0</v>
+        <v>0.0</v>
       </c>
       <c r="F8" s="5">
-        <v>207.0</v>
+        <v>0.0</v>
       </c>
       <c r="G8" s="5">
-        <v>201.0</v>
+        <v>0.0</v>
       </c>
       <c r="H8" s="5">
-        <v>232.0</v>
+        <v>1.0</v>
       </c>
       <c r="I8" s="5">
-        <v>834.0</v>
+        <v>2.0</v>
       </c>
       <c r="J8" s="5">
-        <v>669.0</v>
+        <v>0.0</v>
       </c>
       <c r="K8" s="5">
-        <v>1045.0</v>
+        <v>5.0</v>
       </c>
       <c r="L8" s="5">
-        <v>3234.0</v>
+        <v>13.0</v>
       </c>
       <c r="M8" s="3">
-        <v>6784.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="9">
@@ -2927,37 +2505,37 @@
         <v>14</v>
       </c>
       <c r="C9" s="8">
-        <v>189.0</v>
+        <v>0.0</v>
       </c>
       <c r="D9" s="8">
-        <v>164.0</v>
+        <v>0.0</v>
       </c>
       <c r="E9" s="8">
-        <v>231.0</v>
+        <v>0.0</v>
       </c>
       <c r="F9" s="8">
-        <v>208.0</v>
+        <v>0.0</v>
       </c>
       <c r="G9" s="8">
-        <v>257.0</v>
+        <v>0.0</v>
       </c>
       <c r="H9" s="8">
-        <v>415.0</v>
+        <v>0.0</v>
       </c>
       <c r="I9" s="8">
-        <v>3342.0</v>
+        <v>22.0</v>
       </c>
       <c r="J9" s="8">
-        <v>4276.0</v>
+        <v>9.0</v>
       </c>
       <c r="K9" s="8">
-        <v>2978.0</v>
+        <v>4.0</v>
       </c>
       <c r="L9" s="8">
-        <v>3908.0</v>
+        <v>8.0</v>
       </c>
       <c r="M9" s="6">
-        <v>15968.0</v>
+        <v>43.0</v>
       </c>
     </row>
   </sheetData>
@@ -2974,401 +2552,14 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.43"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11">
-        <v>45383.0</v>
-      </c>
-      <c r="F1" s="11">
-        <v>45540.0</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>2020.0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6">
-        <v>2020.0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>8.0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>2021.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6">
-        <v>2021.0</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="K5" s="8">
-        <v>22.0</v>
-      </c>
-      <c r="L5" s="8">
-        <v>4.0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>27.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3">
-        <v>2022.0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>11.0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6">
-        <v>2022.0</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>6.0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>11.0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>23.0</v>
-      </c>
-      <c r="L7" s="8">
-        <v>13.0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>53.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <v>2023.0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>18.0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6">
-        <v>2023.0</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>16.0</v>
-      </c>
-      <c r="J9" s="8">
-        <v>9.0</v>
-      </c>
-      <c r="K9" s="8">
-        <v>8.0</v>
-      </c>
-      <c r="L9" s="8">
-        <v>10.0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>43.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="26" width="8.43"/>
+    <col customWidth="1" min="1" max="25" width="8.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3420,37 +2611,37 @@
         <v>13</v>
       </c>
       <c r="C2" s="5">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c r="D2" s="5">
-        <v>0.0</v>
+        <v>12.0</v>
       </c>
       <c r="E2" s="5">
-        <v>0.0</v>
+        <v>59.0</v>
       </c>
       <c r="F2" s="5">
-        <v>0.0</v>
+        <v>94.0</v>
       </c>
       <c r="G2" s="5">
-        <v>0.0</v>
+        <v>81.0</v>
       </c>
       <c r="H2" s="5">
-        <v>0.0</v>
+        <v>71.0</v>
       </c>
       <c r="I2" s="5">
-        <v>0.0</v>
+        <v>173.0</v>
       </c>
       <c r="J2" s="5">
-        <v>0.0</v>
+        <v>188.0</v>
       </c>
       <c r="K2" s="5">
-        <v>0.0</v>
+        <v>363.0</v>
       </c>
       <c r="L2" s="5">
-        <v>0.0</v>
+        <v>868.0</v>
       </c>
       <c r="M2" s="3">
-        <v>0.0</v>
+        <v>1914.0</v>
       </c>
     </row>
     <row r="3">
@@ -3461,37 +2652,37 @@
         <v>14</v>
       </c>
       <c r="C3" s="8">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="D3" s="8">
-        <v>0.0</v>
+        <v>13.0</v>
       </c>
       <c r="E3" s="8">
-        <v>0.0</v>
+        <v>71.0</v>
       </c>
       <c r="F3" s="8">
-        <v>0.0</v>
+        <v>72.0</v>
       </c>
       <c r="G3" s="8">
-        <v>0.0</v>
+        <v>91.0</v>
       </c>
       <c r="H3" s="8">
-        <v>0.0</v>
+        <v>78.0</v>
       </c>
       <c r="I3" s="8">
-        <v>0.0</v>
+        <v>636.0</v>
       </c>
       <c r="J3" s="8">
-        <v>0.0</v>
+        <v>669.0</v>
       </c>
       <c r="K3" s="8">
-        <v>0.0</v>
+        <v>601.0</v>
       </c>
       <c r="L3" s="8">
-        <v>0.0</v>
+        <v>747.0</v>
       </c>
       <c r="M3" s="6">
-        <v>0.0</v>
+        <v>2992.0</v>
       </c>
     </row>
     <row r="4">
@@ -3502,37 +2693,37 @@
         <v>13</v>
       </c>
       <c r="C4" s="5">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="D4" s="5">
-        <v>0.0</v>
+        <v>23.0</v>
       </c>
       <c r="E4" s="5">
-        <v>0.0</v>
+        <v>206.0</v>
       </c>
       <c r="F4" s="5">
-        <v>0.0</v>
+        <v>261.0</v>
       </c>
       <c r="G4" s="5">
-        <v>0.0</v>
+        <v>280.0</v>
       </c>
       <c r="H4" s="5">
-        <v>0.0</v>
+        <v>126.0</v>
       </c>
       <c r="I4" s="5">
-        <v>0.0</v>
+        <v>468.0</v>
       </c>
       <c r="J4" s="5">
-        <v>0.0</v>
+        <v>546.0</v>
       </c>
       <c r="K4" s="5">
-        <v>0.0</v>
+        <v>704.0</v>
       </c>
       <c r="L4" s="5">
-        <v>0.0</v>
+        <v>1689.0</v>
       </c>
       <c r="M4" s="3">
-        <v>0.0</v>
+        <v>4338.0</v>
       </c>
     </row>
     <row r="5">
@@ -3543,37 +2734,37 @@
         <v>14</v>
       </c>
       <c r="C5" s="8">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
       <c r="D5" s="8">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="E5" s="8">
-        <v>0.0</v>
+        <v>198.0</v>
       </c>
       <c r="F5" s="8">
-        <v>0.0</v>
+        <v>241.0</v>
       </c>
       <c r="G5" s="8">
-        <v>0.0</v>
+        <v>261.0</v>
       </c>
       <c r="H5" s="8">
-        <v>0.0</v>
+        <v>259.0</v>
       </c>
       <c r="I5" s="8">
-        <v>0.0</v>
+        <v>1911.0</v>
       </c>
       <c r="J5" s="8">
-        <v>0.0</v>
+        <v>2516.0</v>
       </c>
       <c r="K5" s="8">
-        <v>0.0</v>
+        <v>1773.0</v>
       </c>
       <c r="L5" s="8">
-        <v>0.0</v>
+        <v>2144.0</v>
       </c>
       <c r="M5" s="6">
-        <v>0.0</v>
+        <v>9388.0</v>
       </c>
     </row>
     <row r="6">
@@ -3584,37 +2775,37 @@
         <v>13</v>
       </c>
       <c r="C6" s="5">
-        <v>0.0</v>
+        <v>45.0</v>
       </c>
       <c r="D6" s="5">
-        <v>0.0</v>
+        <v>31.0</v>
       </c>
       <c r="E6" s="5">
-        <v>1.0</v>
+        <v>351.0</v>
       </c>
       <c r="F6" s="5">
-        <v>0.0</v>
+        <v>428.0</v>
       </c>
       <c r="G6" s="5">
-        <v>0.0</v>
+        <v>408.0</v>
       </c>
       <c r="H6" s="5">
-        <v>0.0</v>
+        <v>302.0</v>
       </c>
       <c r="I6" s="5">
-        <v>0.0</v>
+        <v>950.0</v>
       </c>
       <c r="J6" s="5">
-        <v>0.0</v>
+        <v>770.0</v>
       </c>
       <c r="K6" s="5">
-        <v>0.0</v>
+        <v>1104.0</v>
       </c>
       <c r="L6" s="5">
-        <v>0.0</v>
+        <v>3605.0</v>
       </c>
       <c r="M6" s="3">
-        <v>1.0</v>
+        <v>7994.0</v>
       </c>
     </row>
     <row r="7">
@@ -3625,37 +2816,37 @@
         <v>14</v>
       </c>
       <c r="C7" s="8">
-        <v>0.0</v>
+        <v>71.0</v>
       </c>
       <c r="D7" s="8">
-        <v>0.0</v>
+        <v>76.0</v>
       </c>
       <c r="E7" s="8">
-        <v>0.0</v>
+        <v>456.0</v>
       </c>
       <c r="F7" s="8">
-        <v>0.0</v>
+        <v>308.0</v>
       </c>
       <c r="G7" s="8">
-        <v>0.0</v>
+        <v>408.0</v>
       </c>
       <c r="H7" s="8">
-        <v>0.0</v>
+        <v>314.0</v>
       </c>
       <c r="I7" s="8">
-        <v>0.0</v>
+        <v>3315.0</v>
       </c>
       <c r="J7" s="8">
-        <v>0.0</v>
+        <v>4577.0</v>
       </c>
       <c r="K7" s="8">
-        <v>0.0</v>
+        <v>3760.0</v>
       </c>
       <c r="L7" s="8">
-        <v>0.0</v>
+        <v>4668.0</v>
       </c>
       <c r="M7" s="6">
-        <v>0.0</v>
+        <v>17953.0</v>
       </c>
     </row>
     <row r="8">
@@ -3666,37 +2857,37 @@
         <v>13</v>
       </c>
       <c r="C8" s="5">
-        <v>0.0</v>
+        <v>76.0</v>
       </c>
       <c r="D8" s="5">
-        <v>0.0</v>
+        <v>68.0</v>
       </c>
       <c r="E8" s="5">
-        <v>0.0</v>
+        <v>218.0</v>
       </c>
       <c r="F8" s="5">
-        <v>0.0</v>
+        <v>207.0</v>
       </c>
       <c r="G8" s="5">
-        <v>0.0</v>
+        <v>201.0</v>
       </c>
       <c r="H8" s="5">
-        <v>0.0</v>
+        <v>232.0</v>
       </c>
       <c r="I8" s="5">
-        <v>0.0</v>
+        <v>834.0</v>
       </c>
       <c r="J8" s="5">
-        <v>0.0</v>
+        <v>669.0</v>
       </c>
       <c r="K8" s="5">
-        <v>0.0</v>
+        <v>1045.0</v>
       </c>
       <c r="L8" s="5">
-        <v>0.0</v>
+        <v>3234.0</v>
       </c>
       <c r="M8" s="3">
-        <v>0.0</v>
+        <v>6784.0</v>
       </c>
     </row>
     <row r="9">
@@ -3707,817 +2898,46 @@
         <v>14</v>
       </c>
       <c r="C9" s="8">
-        <v>0.0</v>
+        <v>189.0</v>
       </c>
       <c r="D9" s="8">
-        <v>0.0</v>
+        <v>164.0</v>
       </c>
       <c r="E9" s="8">
-        <v>0.0</v>
+        <v>231.0</v>
       </c>
       <c r="F9" s="8">
-        <v>0.0</v>
+        <v>208.0</v>
       </c>
       <c r="G9" s="8">
-        <v>0.0</v>
+        <v>257.0</v>
       </c>
       <c r="H9" s="8">
-        <v>0.0</v>
+        <v>415.0</v>
       </c>
       <c r="I9" s="8">
-        <v>0.0</v>
+        <v>3342.0</v>
       </c>
       <c r="J9" s="8">
-        <v>0.0</v>
+        <v>4276.0</v>
       </c>
       <c r="K9" s="8">
-        <v>0.0</v>
+        <v>2978.0</v>
       </c>
       <c r="L9" s="8">
-        <v>0.0</v>
+        <v>3908.0</v>
       </c>
       <c r="M9" s="6">
-        <v>0.0</v>
+        <v>15968.0</v>
       </c>
     </row>
   </sheetData>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="26" width="8.57"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11">
-        <v>45383.0</v>
-      </c>
-      <c r="F1" s="11">
-        <v>45540.0</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>2020.0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6">
-        <v>2020.0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>2021.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6">
-        <v>2021.0</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="K5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="L5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3">
-        <v>2022.0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6">
-        <v>2022.0</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="L7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <v>2023.0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6">
-        <v>2023.0</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="K9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="L9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="26" width="8.43"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11">
-        <v>45383.0</v>
-      </c>
-      <c r="F1" s="11">
-        <v>45540.0</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="3">
-        <v>2020.0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I2" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K2" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="L2" s="5">
-        <v>3.0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="6">
-        <v>2020.0</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H3" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="I3" s="8">
-        <v>1.0</v>
-      </c>
-      <c r="J3" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="K3" s="8">
-        <v>9.0</v>
-      </c>
-      <c r="L3" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3">
-        <v>2021.0</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="M4" s="3">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6">
-        <v>2021.0</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I5" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="J5" s="8">
-        <v>2.0</v>
-      </c>
-      <c r="K5" s="8">
-        <v>22.0</v>
-      </c>
-      <c r="L5" s="8">
-        <v>6.0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3">
-        <v>2022.0</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>1.0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>12.0</v>
-      </c>
-      <c r="M6" s="3">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6">
-        <v>2022.0</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I7" s="8">
-        <v>12.0</v>
-      </c>
-      <c r="J7" s="8">
-        <v>16.0</v>
-      </c>
-      <c r="K7" s="8">
-        <v>23.0</v>
-      </c>
-      <c r="L7" s="8">
-        <v>14.0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>65.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3">
-        <v>2023.0</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>6.0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>21.0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>35.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="6">
-        <v>2023.0</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="I9" s="8">
-        <v>24.0</v>
-      </c>
-      <c r="J9" s="8">
-        <v>12.0</v>
-      </c>
-      <c r="K9" s="8">
-        <v>15.0</v>
-      </c>
-      <c r="L9" s="8">
-        <v>11.0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>62.0</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>